<commit_message>
import only invoicable records import budget name from different column allow import of specific file extensions only error message when import record is incomplete
</commit_message>
<xml_diff>
--- a/budgeteer-aproda-importer/src/test/resources/aproda-testreport.xlsx
+++ b/budgeteer-aproda-importer/src/test/resources/aproda-testreport.xlsx
@@ -17,14 +17,20 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Arbeitspakete!$A$3:$M$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">'Arbeitspakete PM'!$1:$4</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Arbeitspakete PM'!$A$3:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles" vbProcedure="false">'Aufwände gesamt'!$1:$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles" vbProcedure="false">'Aufwände gesamt'!$1:$4</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Aufwände gesamt'!$A$3:$J$3</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Arbeitspakete!$1:$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">Arbeitspakete!$1:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Arbeitspakete!$A$3:$M$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Arbeitspakete!$A$3:$M$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">'Arbeitspakete PM'!$1:$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0" vbProcedure="false">'Arbeitspakete PM'!$1:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Arbeitspakete PM'!$A$3:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles" vbProcedure="false">'Aufwände gesamt'!$1:$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Arbeitspakete PM'!$A$3:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles" vbProcedure="false">'Aufwände gesamt'!$1:$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles_0" vbProcedure="false">'Aufwände gesamt'!$1:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Aufwände gesamt'!$A$3:$J$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Aufwände gesamt'!$A$3:$J$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -72,7 +78,7 @@
     <t>Projektinfrastruktur</t>
   </si>
   <si>
-    <t> </t>
+    <t>Budget</t>
   </si>
   <si>
     <t>Erstellung Entwicklungs-VM</t>
@@ -95,11 +101,12 @@
     <numFmt numFmtId="167" formatCode="#,##0.00&quot;  %&quot;"/>
     <numFmt numFmtId="168" formatCode="#,##0.0&quot; PT&quot;"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -133,12 +140,6 @@
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -236,59 +237,59 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -302,11 +303,46 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <dxfs count="5">
-    <dxf/>
-    <dxf/>
-    <dxf/>
-    <dxf/>
-    <dxf/>
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
   </dxfs>
   <colors>
     <indexedColors>
@@ -376,15 +412,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>597960</xdr:colOff>
+      <xdr:colOff>624960</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>810720</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>6120</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>21960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -399,8 +435,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12366720" y="3600"/>
-          <a:ext cx="2086920" cy="494640"/>
+          <a:off x="12393720" y="3600"/>
+          <a:ext cx="2086560" cy="494280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -420,15 +456,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>546120</xdr:colOff>
+      <xdr:colOff>573120</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1410120</xdr:colOff>
+      <xdr:colOff>1436760</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>21960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -443,8 +479,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7170840" y="3600"/>
-          <a:ext cx="2048400" cy="494640"/>
+          <a:off x="7197840" y="3600"/>
+          <a:ext cx="2048040" cy="494280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -464,15 +500,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>2276640</xdr:colOff>
+      <xdr:colOff>2303640</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>943920</xdr:colOff>
+      <xdr:colOff>970560</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>21960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -487,8 +523,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10369080" y="3600"/>
-          <a:ext cx="2179800" cy="494640"/>
+          <a:off x="10396080" y="3600"/>
+          <a:ext cx="2179440" cy="494280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -506,7 +542,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:M24"/>
@@ -514,7 +550,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="1" sqref="E11 A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="1" sqref="F11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -919,7 +955,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G21"/>
@@ -927,7 +963,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D21" activeCellId="1" sqref="E11 D21"/>
+      <selection pane="bottomLeft" activeCell="D21" activeCellId="1" sqref="F11 D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1138,7 +1174,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J65536"/>
@@ -1146,7 +1182,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Issue #40 (cherry picked from commit fc3fe50)
</commit_message>
<xml_diff>
--- a/budgeteer-aproda-importer/src/test/resources/aproda-testreport.xlsx
+++ b/budgeteer-aproda-importer/src/test/resources/aproda-testreport.xlsx
@@ -1,43 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="372" firstSheet="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="372" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Arbeitspakete" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Arbeitspakete PM" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Aufwände gesamt" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Arbeitspakete" sheetId="1" r:id="rId1"/>
+    <sheet name="Arbeitspakete PM" sheetId="2" r:id="rId2"/>
+    <sheet name="Aufwände gesamt" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Arbeitspakete!$1:$4</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Arbeitspakete!$A$3:$M$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">'Arbeitspakete PM'!$1:$4</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Arbeitspakete PM'!$A$3:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles" vbProcedure="false">'Aufwände gesamt'!$1:$4</definedName>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Aufwände gesamt'!$A$3:$J$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Arbeitspakete!$1:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">Arbeitspakete!$1:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Arbeitspakete!$A$3:$M$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Arbeitspakete!$A$3:$M$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">'Arbeitspakete PM'!$1:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0" vbProcedure="false">'Arbeitspakete PM'!$1:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Arbeitspakete PM'!$A$3:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Arbeitspakete PM'!$A$3:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles" vbProcedure="false">'Aufwände gesamt'!$1:$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles_0" vbProcedure="false">'Aufwände gesamt'!$1:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Aufwände gesamt'!$A$3:$J$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Aufwände gesamt'!$A$3:$J$3</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="0">Arbeitspakete!$A$3:$M$3</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="1">'Arbeitspakete PM'!$A$3:$G$3</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="2">'Aufwände gesamt'!$A$3:$J$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Arbeitspakete!$A$3:$M$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">'Arbeitspakete PM'!$A$3:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2">'Aufwände gesamt'!$A$3:$J$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Arbeitspakete!$1:$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Arbeitspakete PM'!$1:$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Aufwände gesamt'!$1:$3</definedName>
+    <definedName name="Print_Titles_0" localSheetId="0">Arbeitspakete!$1:$4</definedName>
+    <definedName name="Print_Titles_0" localSheetId="1">'Arbeitspakete PM'!$1:$4</definedName>
+    <definedName name="Print_Titles_0" localSheetId="2">'Aufwände gesamt'!$1:$4</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -89,19 +83,29 @@
   <si>
     <t>studentische Hilfskraft</t>
   </si>
+  <si>
+    <t xml:space="preserve">Doe, John </t>
+  </si>
+  <si>
+    <t>Budget1</t>
+  </si>
+  <si>
+    <t>Budget3</t>
+  </si>
+  <si>
+    <t>Roe, Richard</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0&quot; h&quot;"/>
-    <numFmt numFmtId="167" formatCode="#,##0.00&quot;  %&quot;"/>
-    <numFmt numFmtId="168" formatCode="#,##0.0&quot; PT&quot;"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="#,##0.0&quot; h&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00&quot;  %&quot;"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0&quot; PT&quot;"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -109,22 +113,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -137,7 +126,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
@@ -145,7 +134,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -173,177 +162,167 @@
     </fill>
   </fills>
   <borders count="3">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="15">
     <dxf>
       <font>
         <sz val="10"/>
         <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <sz val="10"/>
         <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <sz val="10"/>
         <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <sz val="10"/>
         <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <sz val="10"/>
         <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <name val="Arial"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <name val="Arial"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <name val="Arial"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <name val="Arial"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <name val="Arial"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <name val="Arial"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <name val="Arial"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <name val="Arial"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <name val="Arial"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <name val="Arial"/>
       </font>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -402,13 +381,26 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>10</xdr:col>
@@ -424,11 +416,11 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Picture 1" descr=""/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -452,7 +444,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>5</xdr:col>
@@ -468,11 +460,11 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Picture 1" descr=""/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -496,7 +488,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>6</xdr:col>
@@ -506,17 +498,17 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>970560</xdr:colOff>
+      <xdr:colOff>913410</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>21960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr=""/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -539,37 +531,321 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+  <a:themeElements>
+    <a:clrScheme name="Larissa">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Larissa">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Larissa">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="true"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="1" sqref="F11 A1"/>
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCellId="1" sqref="F11 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.77551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.780612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.780612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.780612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="12.780612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7755102040816"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.780612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.7857142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="12.780612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.780612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="5.7109375"/>
+    <col min="2" max="2" width="20.7109375"/>
+    <col min="3" max="3" width="13.7109375"/>
+    <col min="4" max="4" width="36.7109375"/>
+    <col min="5" max="6" width="12.7109375"/>
+    <col min="7" max="7" width="22.7109375"/>
+    <col min="8" max="8" width="12.7109375"/>
+    <col min="9" max="9" width="15.7109375"/>
+    <col min="10" max="11" width="12.7109375"/>
+    <col min="12" max="12" width="13.7109375"/>
+    <col min="13" max="13" width="11.7109375"/>
+    <col min="14" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -580,10 +856,10 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -598,7 +874,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -613,7 +889,7 @@
       <c r="L4" s="4"/>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -628,7 +904,7 @@
       <c r="L5" s="4"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -643,7 +919,7 @@
       <c r="L6" s="8"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -658,7 +934,7 @@
       <c r="L7" s="4"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -673,7 +949,7 @@
       <c r="L8" s="8"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -688,7 +964,7 @@
       <c r="L9" s="4"/>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -703,7 +979,7 @@
       <c r="L10" s="4"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -718,7 +994,7 @@
       <c r="L11" s="4"/>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -733,7 +1009,7 @@
       <c r="L12" s="4"/>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -748,7 +1024,7 @@
       <c r="L13" s="4"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -763,7 +1039,7 @@
       <c r="L14" s="4"/>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -778,7 +1054,7 @@
       <c r="L15" s="4"/>
       <c r="M15" s="6"/>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -793,7 +1069,7 @@
       <c r="L16" s="8"/>
       <c r="M16" s="6"/>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -808,7 +1084,7 @@
       <c r="L17" s="4"/>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -823,7 +1099,7 @@
       <c r="L18" s="8"/>
       <c r="M18" s="6"/>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -838,7 +1114,7 @@
       <c r="L19" s="4"/>
       <c r="M19" s="6"/>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -853,7 +1129,7 @@
       <c r="L20" s="11"/>
       <c r="M20" s="13"/>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D21" s="15"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
@@ -862,7 +1138,7 @@
       <c r="K21" s="6"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D22" s="15"/>
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
@@ -870,7 +1146,7 @@
       <c r="K22" s="16"/>
       <c r="M22" s="16"/>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D24" s="17"/>
       <c r="E24" s="6"/>
       <c r="J24" s="17"/>
@@ -882,113 +1158,106 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="J4:J21">
-    <cfRule type="cellIs" priority="2" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThan">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="4" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThanOrEqual">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29:J30">
-    <cfRule type="cellIs" priority="5" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="lessThan">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="6" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="7" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="greaterThanOrEqual">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J35:J36">
-    <cfRule type="cellIs" priority="8" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="lessThan">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="10" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="greaterThanOrEqual">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K21">
-    <cfRule type="cellIs" priority="11" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="12" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" dxfId="4" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29:K30">
-    <cfRule type="cellIs" priority="13" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" dxfId="3" priority="13" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="14" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" dxfId="2" priority="14" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35:K36">
-    <cfRule type="cellIs" priority="15" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" dxfId="1" priority="15" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="16" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" dxfId="0" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D21" activeCellId="1" sqref="F11 D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.77551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.780612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.7755102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.780612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.7857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="6.7109375"/>
+    <col min="2" max="2" width="17.7109375"/>
+    <col min="3" max="3" width="14.7109375"/>
+    <col min="4" max="4" width="40.7109375"/>
+    <col min="5" max="5" width="13.7109375"/>
+    <col min="6" max="6" width="16.7109375"/>
+    <col min="7" max="7" width="20.7109375"/>
+    <col min="8" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -997,7 +1266,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1006,7 +1275,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1015,7 +1284,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1024,7 +1293,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1033,7 +1302,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1042,7 +1311,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1051,7 +1320,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1060,7 +1329,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1069,7 +1338,7 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1078,7 +1347,7 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1087,7 +1356,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1096,7 +1365,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1105,7 +1374,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1114,7 +1383,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1123,7 +1392,7 @@
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1132,7 +1401,7 @@
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1141,7 +1410,7 @@
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -1150,7 +1419,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D21" s="15"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
@@ -1160,56 +1429,49 @@
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J65536"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.780612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.780612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="15.7857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="49.7857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.780612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.77551020408163"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="26.7109375"/>
+    <col min="2" max="2" width="10.7109375"/>
+    <col min="3" max="3" width="14.7109375"/>
+    <col min="4" max="4" width="30.7109375"/>
+    <col min="5" max="6" width="15.7109375"/>
+    <col min="7" max="7" width="49.7109375"/>
+    <col min="8" max="8" width="13.7109375"/>
+    <col min="9" max="9" width="6.7109375"/>
+    <col min="10" max="10" width="21.7109375"/>
+    <col min="11" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1241,11 +1503,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="n">
+      <c r="B4" s="5">
         <v>41918</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1263,7 +1525,7 @@
       <c r="G4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="6" t="n">
+      <c r="H4" s="6">
         <v>9</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -1273,11 +1535,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="5">
         <v>41920</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1295,7 +1557,7 @@
       <c r="G5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="6" t="n">
+      <c r="H5" s="6">
         <v>7</v>
       </c>
       <c r="I5" s="4" t="s">
@@ -1305,11 +1567,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="5">
         <v>41925</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1327,7 +1589,7 @@
       <c r="G6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="6" t="n">
+      <c r="H6" s="6">
         <v>7</v>
       </c>
       <c r="I6" s="4" t="s">
@@ -1337,11 +1599,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="5">
         <v>41939</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1359,7 +1621,7 @@
       <c r="G7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="6" t="n">
+      <c r="H7" s="6">
         <v>8</v>
       </c>
       <c r="I7" s="4" t="s">
@@ -1369,11 +1631,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="5">
         <v>41940</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1391,7 +1653,7 @@
       <c r="G8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="6" t="n">
+      <c r="H8" s="6">
         <v>8</v>
       </c>
       <c r="I8" s="4" t="s">
@@ -1401,11 +1663,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5" t="n">
+      <c r="B9" s="5">
         <v>41941</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1423,7 +1685,7 @@
       <c r="G9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="6" t="n">
+      <c r="H9" s="6">
         <v>8.5</v>
       </c>
       <c r="I9" s="4" t="s">
@@ -1433,11 +1695,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="n">
+      <c r="B10" s="5">
         <v>41942</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1455,7 +1717,7 @@
       <c r="G10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="6" t="n">
+      <c r="H10" s="6">
         <v>8.5</v>
       </c>
       <c r="I10" s="4" t="s">
@@ -1465,11 +1727,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="n">
+      <c r="B11" s="5">
         <v>41943</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1487,7 +1749,7 @@
       <c r="G11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="6" t="n">
+      <c r="H11" s="6">
         <v>8</v>
       </c>
       <c r="I11" s="4" t="s">
@@ -1497,28 +1759,781 @@
         <v>16</v>
       </c>
     </row>
-    <row r="1006" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="5">
+        <v>41918</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="6">
+        <v>9</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="5">
+        <v>41920</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="6">
+        <v>7</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="5">
+        <v>41925</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="6">
+        <v>7</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="5">
+        <v>41939</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="6">
+        <v>8</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="5">
+        <v>41940</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="6">
+        <v>8</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="5">
+        <v>41941</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5">
+        <v>41942</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="5">
+        <v>41943</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="6">
+        <v>8</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="5">
+        <v>41918</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="6">
+        <v>9</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="5">
+        <v>41920</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="6">
+        <v>7</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="5">
+        <v>41925</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="6">
+        <v>7</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="5">
+        <v>41939</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="6">
+        <v>8</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="5">
+        <v>41940</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="6">
+        <v>8</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="5">
+        <v>41941</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="5">
+        <v>41942</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="5">
+        <v>41943</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="6">
+        <v>8</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="5">
+        <v>41918</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="6">
+        <v>9</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="5">
+        <v>41920</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="6">
+        <v>7</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="5">
+        <v>41925</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" s="6">
+        <v>7</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="5">
+        <v>41939</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" s="6">
+        <v>8</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="5">
+        <v>41940</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="6">
+        <v>8</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="5">
+        <v>41941</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="5">
+        <v>41942</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="5">
+        <v>41943</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="6">
+        <v>8</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:J3"/>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Issue  #61 (cherry picked from commit a7b021b)
</commit_message>
<xml_diff>
--- a/budgeteer-aproda-importer/src/test/resources/aproda-testreport.xlsx
+++ b/budgeteer-aproda-importer/src/test/resources/aproda-testreport.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>studentische Hilfskraft</t>
+  </si>
+  <si>
+    <t>Nein</t>
   </si>
 </sst>
 </file>
@@ -1430,9 +1433,9 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1748,36 +1751,64 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4">
+        <v>41942</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="H12" s="5">
         <v>9</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="A13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4">
+        <v>41943</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="H13" s="5">
         <v>7</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>16</v>

</xml_diff>